<commit_message>
fearture read pdf uploeaded
</commit_message>
<xml_diff>
--- a/media/excel_outputs/excel_doi_chieu.xlsx
+++ b/media/excel_outputs/excel_doi_chieu.xlsx
@@ -584,7 +584,7 @@
           <t>Mường</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -641,7 +641,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -698,7 +698,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -755,7 +755,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -812,7 +812,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="W6" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -869,7 +869,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="W7" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -926,7 +926,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="W8" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -983,7 +983,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -1040,7 +1040,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>
@@ -1097,7 +1097,7 @@
           <t>Kinh</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>Số: 245 /QĐ-CĐFPL Hà Nội, ngày 18 tháng 08 năm 2022</t>
         </is>

</xml_diff>